<commit_message>
new excel files, m.files
cross validation, test data
</commit_message>
<xml_diff>
--- a/KW/Windows_H2.xlsx
+++ b/KW/Windows_H2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7815" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="H2-1" sheetId="11" r:id="rId1"/>
@@ -618,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R57"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5917,8 +5917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>